<commit_message>
Refining process for getting key details on projects.
</commit_message>
<xml_diff>
--- a/FOIA SAR data/RawHeaderList.xlsx
+++ b/FOIA SAR data/RawHeaderList.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="RawHeaderList" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" calcMode="manual"/>
 </workbook>
 </file>
 
@@ -1917,7 +1917,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -2400,7 +2400,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -2759,11 +2759,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U408"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B367" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N23" sqref="N23"/>
+      <selection pane="bottomRight" activeCell="L400" sqref="L400"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6018,6 +6018,9 @@
       <c r="O143" t="s">
         <v>275</v>
       </c>
+      <c r="U143">
+        <v>2012</v>
+      </c>
     </row>
     <row r="144" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
@@ -6033,7 +6036,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>255</v>
       </c>
@@ -6044,7 +6047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>278</v>
       </c>
@@ -6058,7 +6061,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>260</v>
       </c>
@@ -6104,8 +6107,11 @@
       <c r="O147" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U147">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="148" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>28</v>
       </c>
@@ -6131,7 +6137,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>285</v>
       </c>
@@ -6154,7 +6160,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>286</v>
       </c>
@@ -6174,7 +6180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>287</v>
       </c>
@@ -6197,7 +6203,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>68</v>
       </c>
@@ -6220,7 +6226,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>292</v>
       </c>
@@ -6243,7 +6249,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>293</v>
       </c>
@@ -6266,7 +6272,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>254</v>
       </c>
@@ -6286,7 +6292,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>295</v>
       </c>
@@ -6303,7 +6309,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>299</v>
       </c>
@@ -6314,7 +6320,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>301</v>
       </c>
@@ -6340,7 +6346,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>303</v>
       </c>
@@ -6366,7 +6372,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
         <v>224</v>
       </c>
@@ -7401,6 +7407,9 @@
       <c r="S194" t="s">
         <v>347</v>
       </c>
+      <c r="U194">
+        <v>1999</v>
+      </c>
     </row>
     <row r="195" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
@@ -9215,6 +9224,9 @@
       <c r="O237" t="s">
         <v>444</v>
       </c>
+      <c r="U237">
+        <v>2002</v>
+      </c>
     </row>
     <row r="238" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A238" s="3">
@@ -9432,6 +9444,9 @@
       <c r="O242" t="s">
         <v>380</v>
       </c>
+      <c r="U242">
+        <v>2003</v>
+      </c>
     </row>
     <row r="243" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A243" s="3">
@@ -14306,6 +14321,9 @@
       <c r="O387" t="s">
         <v>252</v>
       </c>
+      <c r="U387">
+        <v>2011</v>
+      </c>
     </row>
     <row r="388" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A388" s="3" t="s">
@@ -14350,6 +14368,9 @@
       <c r="O388" t="s">
         <v>252</v>
       </c>
+      <c r="U388">
+        <v>2011</v>
+      </c>
     </row>
     <row r="389" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A389" s="3" t="s">
@@ -14393,6 +14414,9 @@
       </c>
       <c r="O389" t="s">
         <v>252</v>
+      </c>
+      <c r="U389">
+        <v>2011</v>
       </c>
     </row>
     <row r="390" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>